<commit_message>
Semi_clean exim.rda w/o anytag
</commit_message>
<xml_diff>
--- a/Output/Assistance/DFC/DFC_Assistance.xlsx
+++ b/Output/Assistance/DFC/DFC_Assistance.xlsx
@@ -1509,11 +1509,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="196" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="198" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="197" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="199" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -1554,13 +1555,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="196" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="198" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="197" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="199" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4012,20 +4014,20 @@
       <c r="M2" t="s">
         <v>343</v>
       </c>
-      <c r="N2" s="2" t="n">
+      <c r="N2" s="6" t="n">
         <v>10000000</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="O2" s="6" t="n">
         <v>459500000</v>
       </c>
-      <c r="P2" s="2" t="n">
+      <c r="P2" s="6" t="n">
         <v>400000000</v>
       </c>
-      <c r="Q2" s="2" t="n">
+      <c r="Q2" s="6" t="n">
         <v>3242592249</v>
       </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -4034,22 +4036,22 @@
       <c r="M3" t="s">
         <v>485</v>
       </c>
-      <c r="N3" s="2" t="str">
+      <c r="N3" s="6" t="str">
         <f>Sum(N2:N2)</f>
       </c>
-      <c r="O3" s="2" t="str">
+      <c r="O3" s="6" t="str">
         <f>Sum(O2:O2)</f>
       </c>
-      <c r="P3" s="2" t="str">
+      <c r="P3" s="6" t="str">
         <f>Sum(P2:P2)</f>
       </c>
-      <c r="Q3" s="2" t="str">
+      <c r="Q3" s="6" t="str">
         <f>Sum(Q2:Q2)</f>
       </c>
-      <c r="R3" s="2" t="str">
+      <c r="R3" s="6" t="str">
         <f>Sum(R2:R2)</f>
       </c>
-      <c r="S3" s="2"/>
+      <c r="S3" s="6"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -4078,31 +4080,31 @@
       <c r="M7" t="s">
         <v>343</v>
       </c>
-      <c r="N7" s="2" t="n">
+      <c r="N7" s="6" t="n">
         <v>10000000</v>
       </c>
-      <c r="O7" s="2" t="n">
+      <c r="O7" s="6" t="n">
         <v>549875454.765218</v>
       </c>
-      <c r="P7" s="2" t="n">
+      <c r="P7" s="6" t="n">
         <v>484513733.175898</v>
       </c>
-      <c r="Q7" s="2" t="n">
+      <c r="Q7" s="6" t="n">
         <v>3817329986.46603</v>
       </c>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <f>M8</f>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Multi-year experiments and financing.
</commit_message>
<xml_diff>
--- a/Output/Assistance/DFC/DFC_Assistance.xlsx
+++ b/Output/Assistance/DFC/DFC_Assistance.xlsx
@@ -1509,11 +1509,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="199" formatCode="0.00,,,&quot;B&quot;"/>
+  <numFmts count="5">
+    <numFmt numFmtId="201" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="198" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="200" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="202" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -1554,13 +1555,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="199" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="201" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="198" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="200" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="202" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4385,11 +4387,11 @@
       <c r="M2" t="s">
         <v>343</v>
       </c>
-      <c r="N2" s="5" t="n">
+      <c r="N2" s="6" t="n">
         <v>4112092249</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -4398,13 +4400,13 @@
       <c r="M3" t="s">
         <v>485</v>
       </c>
-      <c r="N3" s="5" t="str">
+      <c r="N3" s="6" t="str">
         <f>Sum(N2:N2)</f>
       </c>
-      <c r="O3" s="5" t="str">
+      <c r="O3" s="6" t="str">
         <f>Sum(O2:O2)</f>
       </c>
-      <c r="P3" s="5"/>
+      <c r="P3" s="6"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -4424,19 +4426,19 @@
       <c r="M7" t="s">
         <v>343</v>
       </c>
-      <c r="N7" s="5" t="n">
+      <c r="N7" s="6" t="n">
         <v>4861719174.40714</v>
       </c>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <f>M8</f>
       </c>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FutureG to modern telecom
</commit_message>
<xml_diff>
--- a/Output/Assistance/DFC/DFC_Assistance.xlsx
+++ b/Output/Assistance/DFC/DFC_Assistance.xlsx
@@ -1509,12 +1509,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
-    <numFmt numFmtId="205" formatCode="0.00,,,&quot;B&quot;"/>
+  <numFmts count="4">
+    <numFmt numFmtId="206" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="203" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="202" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="206" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -1555,14 +1554,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="205" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="206" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="203" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="202" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="206" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4014,20 +4012,20 @@
       <c r="M2" t="s">
         <v>343</v>
       </c>
-      <c r="N2" s="6" t="n">
+      <c r="N2" s="2" t="n">
         <v>10000000</v>
       </c>
-      <c r="O2" s="6" t="n">
+      <c r="O2" s="2" t="n">
         <v>459500000</v>
       </c>
-      <c r="P2" s="6" t="n">
+      <c r="P2" s="2" t="n">
         <v>400000000</v>
       </c>
-      <c r="Q2" s="6" t="n">
+      <c r="Q2" s="2" t="n">
         <v>3242592249</v>
       </c>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -4036,22 +4034,22 @@
       <c r="M3" t="s">
         <v>485</v>
       </c>
-      <c r="N3" s="6" t="str">
+      <c r="N3" s="2" t="str">
         <f>Sum(N2:N2)</f>
       </c>
-      <c r="O3" s="6" t="str">
+      <c r="O3" s="2" t="str">
         <f>Sum(O2:O2)</f>
       </c>
-      <c r="P3" s="6" t="str">
+      <c r="P3" s="2" t="str">
         <f>Sum(P2:P2)</f>
       </c>
-      <c r="Q3" s="6" t="str">
+      <c r="Q3" s="2" t="str">
         <f>Sum(Q2:Q2)</f>
       </c>
-      <c r="R3" s="6" t="str">
+      <c r="R3" s="2" t="str">
         <f>Sum(R2:R2)</f>
       </c>
-      <c r="S3" s="6"/>
+      <c r="S3" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -4080,31 +4078,31 @@
       <c r="M7" t="s">
         <v>343</v>
       </c>
-      <c r="N7" s="6" t="n">
+      <c r="N7" s="2" t="n">
         <v>10000000</v>
       </c>
-      <c r="O7" s="6" t="n">
+      <c r="O7" s="2" t="n">
         <v>549875454.765218</v>
       </c>
-      <c r="P7" s="6" t="n">
+      <c r="P7" s="2" t="n">
         <v>484513733.175898</v>
       </c>
-      <c r="Q7" s="6" t="n">
+      <c r="Q7" s="2" t="n">
         <v>3817329986.46603</v>
       </c>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <f>M8</f>
       </c>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Partner region in agency_aggregate
</commit_message>
<xml_diff>
--- a/Output/Assistance/DFC/DFC_Assistance.xlsx
+++ b/Output/Assistance/DFC/DFC_Assistance.xlsx
@@ -1510,7 +1510,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="206" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="207" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="203" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="202" formatCode="0.00,,,&quot;B&quot;"/>
@@ -1557,7 +1557,7 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="206" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="207" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="203" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="202" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -1885,7 +1885,7 @@
         <v>251</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>252</v>
+        <v>490</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>253</v>

</xml_diff>

<commit_message>
Loan axis title fixes.
</commit_message>
<xml_diff>
--- a/Output/Assistance/DFC/DFC_Assistance.xlsx
+++ b/Output/Assistance/DFC/DFC_Assistance.xlsx
@@ -1523,15 +1523,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
-    <numFmt numFmtId="229" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="234" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="208" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="212" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="226" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="227" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="232" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="235" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="233" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="211" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="233" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="236" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -1575,15 +1575,15 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="229" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="234" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="208" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="212" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="226" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="227" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="232" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="235" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="233" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="211" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="233" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="236" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4472,11 +4472,11 @@
       <c r="M2" t="s">
         <v>343</v>
       </c>
-      <c r="N2" s="7" t="n">
+      <c r="N2" s="10" t="n">
         <v>4112092249</v>
       </c>
-      <c r="O2" s="7"/>
-      <c r="P2" s="7"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -4485,13 +4485,13 @@
       <c r="M3" t="s">
         <v>485</v>
       </c>
-      <c r="N3" s="7" t="str">
+      <c r="N3" s="10" t="str">
         <f>Sum(N2:N2)</f>
       </c>
-      <c r="O3" s="7" t="str">
+      <c r="O3" s="10" t="str">
         <f>Sum(O2:O2)</f>
       </c>
-      <c r="P3" s="7"/>
+      <c r="P3" s="10"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -4511,19 +4511,19 @@
       <c r="M7" t="s">
         <v>343</v>
       </c>
-      <c r="N7" s="7" t="n">
+      <c r="N7" s="10" t="n">
         <v>4861719174.40714</v>
       </c>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <f>M8</f>
       </c>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4581,31 +4581,31 @@
       <c r="M2" t="s">
         <v>343</v>
       </c>
-      <c r="N2" s="10" t="n">
+      <c r="N2" s="8" t="n">
         <v>1510209553</v>
       </c>
-      <c r="O2" s="10" t="n">
+      <c r="O2" s="8" t="n">
         <v>19782159</v>
       </c>
-      <c r="P2" s="10" t="n">
+      <c r="P2" s="8" t="n">
         <v>1237111264</v>
       </c>
-      <c r="Q2" s="10" t="n">
+      <c r="Q2" s="8" t="n">
         <v>340000000</v>
       </c>
-      <c r="R2" s="10" t="n">
+      <c r="R2" s="8" t="n">
         <v>407497812</v>
       </c>
-      <c r="S2" s="10" t="n">
+      <c r="S2" s="8" t="n">
         <v>527500000</v>
       </c>
-      <c r="T2" s="10" t="n">
+      <c r="T2" s="8" t="n">
         <v>69991461</v>
       </c>
-      <c r="U2" s="10" t="n">
+      <c r="U2" s="8" t="n">
         <v>69991461</v>
       </c>
-      <c r="V2" s="10"/>
+      <c r="V2" s="8"/>
       <c r="W2" s="9"/>
     </row>
     <row r="3">
@@ -4615,31 +4615,31 @@
       <c r="M3" t="s">
         <v>485</v>
       </c>
-      <c r="N3" s="10" t="str">
+      <c r="N3" s="8" t="str">
         <f>Sum(N2:N2)</f>
       </c>
-      <c r="O3" s="10" t="str">
+      <c r="O3" s="8" t="str">
         <f>Sum(O2:O2)</f>
       </c>
-      <c r="P3" s="10" t="str">
+      <c r="P3" s="8" t="str">
         <f>Sum(P2:P2)</f>
       </c>
-      <c r="Q3" s="10" t="str">
+      <c r="Q3" s="8" t="str">
         <f>Sum(Q2:Q2)</f>
       </c>
-      <c r="R3" s="10" t="str">
+      <c r="R3" s="8" t="str">
         <f>Sum(R2:R2)</f>
       </c>
-      <c r="S3" s="10" t="str">
+      <c r="S3" s="8" t="str">
         <f>Sum(S2:S2)</f>
       </c>
-      <c r="T3" s="10" t="str">
+      <c r="T3" s="8" t="str">
         <f>Sum(T2:T2)</f>
       </c>
-      <c r="U3" s="10" t="str">
+      <c r="U3" s="8" t="str">
         <f>Sum(U2:U2)</f>
       </c>
-      <c r="V3" s="10" t="str">
+      <c r="V3" s="8" t="str">
         <f>Sum(V2:V2)</f>
       </c>
       <c r="W3" s="9"/>
@@ -4683,46 +4683,46 @@
       <c r="M7" t="s">
         <v>343</v>
       </c>
-      <c r="N7" s="10" t="n">
+      <c r="N7" s="8" t="n">
         <v>1712884905.91091</v>
       </c>
-      <c r="O7" s="10" t="n">
+      <c r="O7" s="8" t="n">
         <v>24555706.2249625</v>
       </c>
-      <c r="P7" s="10" t="n">
+      <c r="P7" s="8" t="n">
         <v>1444835352.09659</v>
       </c>
-      <c r="Q7" s="10" t="n">
+      <c r="Q7" s="8" t="n">
         <v>417162347.149875</v>
       </c>
-      <c r="R7" s="10" t="n">
+      <c r="R7" s="8" t="n">
         <v>539668692.22086</v>
       </c>
-      <c r="S7" s="10" t="n">
+      <c r="S7" s="8" t="n">
         <v>639166858.749091</v>
       </c>
-      <c r="T7" s="10" t="n">
+      <c r="T7" s="8" t="n">
         <v>83445312.0548523</v>
       </c>
-      <c r="U7" s="10" t="n">
+      <c r="U7" s="8" t="n">
         <v>83445312.0548523</v>
       </c>
-      <c r="V7" s="10"/>
+      <c r="V7" s="8"/>
       <c r="W7" s="9"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <f>M8</f>
       </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
       <c r="W8" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing unlabeled and other last details.
</commit_message>
<xml_diff>
--- a/Output/Assistance/DFC/DFC_Assistance.xlsx
+++ b/Output/Assistance/DFC/DFC_Assistance.xlsx
@@ -1523,15 +1523,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
-    <numFmt numFmtId="234" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="257" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="208" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="212" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="252" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="226" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="235" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="233" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="236" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="211" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="236" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="247" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="258" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -1575,15 +1575,15 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="234" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="257" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="208" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="212" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="252" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="226" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="235" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="233" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="236" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="211" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="236" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="247" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="258" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4028,13 +4028,13 @@
         <v>255</v>
       </c>
       <c r="R1" t="s">
-        <v>494</v>
+        <v>256</v>
       </c>
       <c r="S1" t="s">
-        <v>362</v>
+        <v>492</v>
       </c>
       <c r="T1" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="U1" t="s">
         <v>290</v>
@@ -4047,31 +4047,31 @@
       <c r="M2" t="s">
         <v>343</v>
       </c>
-      <c r="N2" s="2" t="n">
+      <c r="N2" s="10" t="n">
         <v>10000000</v>
       </c>
-      <c r="O2" s="2" t="n">
+      <c r="O2" s="10" t="n">
         <v>459500000</v>
       </c>
-      <c r="P2" s="2" t="n">
+      <c r="P2" s="10" t="n">
         <v>400000000</v>
       </c>
-      <c r="Q2" s="2" t="n">
+      <c r="Q2" s="10" t="n">
         <v>3242592249</v>
       </c>
-      <c r="R2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" s="2" t="n">
-        <v>340000000</v>
+      <c r="R2" s="10" t="n">
+        <v>407497812</v>
+      </c>
+      <c r="S2" s="10" t="n">
+        <v>527500000</v>
       </c>
       <c r="T2" s="4" t="n">
-        <v>527500000</v>
-      </c>
-      <c r="U2" s="3" t="n">
         <v>69991461</v>
       </c>
-      <c r="V2" s="3"/>
+      <c r="U2" s="4" t="n">
+        <v>69991461</v>
+      </c>
+      <c r="V2" s="4"/>
       <c r="W2" s="3"/>
     </row>
     <row r="3">
@@ -4081,31 +4081,31 @@
       <c r="M3" t="s">
         <v>485</v>
       </c>
-      <c r="N3" s="2" t="str">
+      <c r="N3" s="10" t="str">
         <f>Sum(N2:N2)</f>
       </c>
-      <c r="O3" s="2" t="str">
+      <c r="O3" s="10" t="str">
         <f>Sum(O2:O2)</f>
       </c>
-      <c r="P3" s="2" t="str">
+      <c r="P3" s="10" t="str">
         <f>Sum(P2:P2)</f>
       </c>
-      <c r="Q3" s="2" t="str">
+      <c r="Q3" s="10" t="str">
         <f>Sum(Q2:Q2)</f>
       </c>
-      <c r="R3" s="2" t="str">
+      <c r="R3" s="10" t="str">
         <f>Sum(R2:R2)</f>
       </c>
-      <c r="S3" s="2" t="str">
+      <c r="S3" s="10" t="str">
         <f>Sum(S2:S2)</f>
       </c>
       <c r="T3" s="4" t="str">
         <f>Sum(T2:T2)</f>
       </c>
-      <c r="U3" s="3" t="str">
+      <c r="U3" s="4" t="str">
         <f>Sum(U2:U2)</f>
       </c>
-      <c r="V3" s="3" t="str">
+      <c r="V3" s="4" t="str">
         <f>Sum(V2:V2)</f>
       </c>
       <c r="W3" s="3"/>
@@ -4130,13 +4130,13 @@
         <v>255</v>
       </c>
       <c r="R6" t="s">
-        <v>494</v>
+        <v>256</v>
       </c>
       <c r="S6" t="s">
-        <v>362</v>
+        <v>492</v>
       </c>
       <c r="T6" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="U6" t="s">
         <v>290</v>
@@ -4149,46 +4149,46 @@
       <c r="M7" t="s">
         <v>343</v>
       </c>
-      <c r="N7" s="2" t="n">
+      <c r="N7" s="10" t="n">
         <v>10000000</v>
       </c>
-      <c r="O7" s="2" t="n">
+      <c r="O7" s="10" t="n">
         <v>549875454.765218</v>
       </c>
-      <c r="P7" s="2" t="n">
+      <c r="P7" s="10" t="n">
         <v>484513733.175898</v>
       </c>
-      <c r="Q7" s="2" t="n">
+      <c r="Q7" s="10" t="n">
         <v>3817329986.46603</v>
       </c>
-      <c r="R7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="2" t="n">
-        <v>417162347.149875</v>
+      <c r="R7" s="10" t="n">
+        <v>539668692.22086</v>
+      </c>
+      <c r="S7" s="10" t="n">
+        <v>639166858.749091</v>
       </c>
       <c r="T7" s="4" t="n">
-        <v>639166858.749091</v>
-      </c>
-      <c r="U7" s="3" t="n">
         <v>83445312.0548523</v>
       </c>
-      <c r="V7" s="3"/>
+      <c r="U7" s="4" t="n">
+        <v>83445312.0548523</v>
+      </c>
+      <c r="V7" s="4"/>
       <c r="W7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <f>M8</f>
       </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
       <c r="T8" s="4"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
       <c r="W8" s="3"/>
     </row>
   </sheetData>
@@ -4472,11 +4472,11 @@
       <c r="M2" t="s">
         <v>343</v>
       </c>
-      <c r="N2" s="10" t="n">
+      <c r="N2" s="7" t="n">
         <v>4112092249</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -4485,13 +4485,13 @@
       <c r="M3" t="s">
         <v>485</v>
       </c>
-      <c r="N3" s="10" t="str">
+      <c r="N3" s="7" t="str">
         <f>Sum(N2:N2)</f>
       </c>
-      <c r="O3" s="10" t="str">
+      <c r="O3" s="7" t="str">
         <f>Sum(O2:O2)</f>
       </c>
-      <c r="P3" s="10"/>
+      <c r="P3" s="7"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -4511,19 +4511,19 @@
       <c r="M7" t="s">
         <v>343</v>
       </c>
-      <c r="N7" s="10" t="n">
+      <c r="N7" s="7" t="n">
         <v>4861719174.40714</v>
       </c>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <f>M8</f>
       </c>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4581,32 +4581,32 @@
       <c r="M2" t="s">
         <v>343</v>
       </c>
-      <c r="N2" s="8" t="n">
+      <c r="N2" s="9" t="n">
         <v>1510209553</v>
       </c>
-      <c r="O2" s="8" t="n">
+      <c r="O2" s="9" t="n">
         <v>19782159</v>
       </c>
-      <c r="P2" s="8" t="n">
+      <c r="P2" s="9" t="n">
         <v>1237111264</v>
       </c>
-      <c r="Q2" s="8" t="n">
+      <c r="Q2" s="9" t="n">
         <v>340000000</v>
       </c>
-      <c r="R2" s="8" t="n">
+      <c r="R2" s="9" t="n">
         <v>407497812</v>
       </c>
-      <c r="S2" s="8" t="n">
+      <c r="S2" s="9" t="n">
         <v>527500000</v>
       </c>
-      <c r="T2" s="8" t="n">
+      <c r="T2" s="9" t="n">
         <v>69991461</v>
       </c>
-      <c r="U2" s="8" t="n">
+      <c r="U2" s="9" t="n">
         <v>69991461</v>
       </c>
-      <c r="V2" s="8"/>
-      <c r="W2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="8"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -4615,34 +4615,34 @@
       <c r="M3" t="s">
         <v>485</v>
       </c>
-      <c r="N3" s="8" t="str">
+      <c r="N3" s="9" t="str">
         <f>Sum(N2:N2)</f>
       </c>
-      <c r="O3" s="8" t="str">
+      <c r="O3" s="9" t="str">
         <f>Sum(O2:O2)</f>
       </c>
-      <c r="P3" s="8" t="str">
+      <c r="P3" s="9" t="str">
         <f>Sum(P2:P2)</f>
       </c>
-      <c r="Q3" s="8" t="str">
+      <c r="Q3" s="9" t="str">
         <f>Sum(Q2:Q2)</f>
       </c>
-      <c r="R3" s="8" t="str">
+      <c r="R3" s="9" t="str">
         <f>Sum(R2:R2)</f>
       </c>
-      <c r="S3" s="8" t="str">
+      <c r="S3" s="9" t="str">
         <f>Sum(S2:S2)</f>
       </c>
-      <c r="T3" s="8" t="str">
+      <c r="T3" s="9" t="str">
         <f>Sum(T2:T2)</f>
       </c>
-      <c r="U3" s="8" t="str">
+      <c r="U3" s="9" t="str">
         <f>Sum(U2:U2)</f>
       </c>
-      <c r="V3" s="8" t="str">
+      <c r="V3" s="9" t="str">
         <f>Sum(V2:V2)</f>
       </c>
-      <c r="W3" s="9"/>
+      <c r="W3" s="8"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -4683,47 +4683,47 @@
       <c r="M7" t="s">
         <v>343</v>
       </c>
-      <c r="N7" s="8" t="n">
+      <c r="N7" s="9" t="n">
         <v>1712884905.91091</v>
       </c>
-      <c r="O7" s="8" t="n">
+      <c r="O7" s="9" t="n">
         <v>24555706.2249625</v>
       </c>
-      <c r="P7" s="8" t="n">
+      <c r="P7" s="9" t="n">
         <v>1444835352.09659</v>
       </c>
-      <c r="Q7" s="8" t="n">
+      <c r="Q7" s="9" t="n">
         <v>417162347.149875</v>
       </c>
-      <c r="R7" s="8" t="n">
+      <c r="R7" s="9" t="n">
         <v>539668692.22086</v>
       </c>
-      <c r="S7" s="8" t="n">
+      <c r="S7" s="9" t="n">
         <v>639166858.749091</v>
       </c>
-      <c r="T7" s="8" t="n">
+      <c r="T7" s="9" t="n">
         <v>83445312.0548523</v>
       </c>
-      <c r="U7" s="8" t="n">
+      <c r="U7" s="9" t="n">
         <v>83445312.0548523</v>
       </c>
-      <c r="V7" s="8"/>
-      <c r="W7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="8"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <f>M8</f>
       </c>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="T8" s="8"/>
-      <c r="U8" s="8"/>
-      <c r="V8" s="8"/>
-      <c r="W8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>